<commit_message>
2022/12/23 구현완료, API 추가
</commit_message>
<xml_diff>
--- a/API/API 설계 조주영.xlsx
+++ b/API/API 설계 조주영.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
   <si>
     <t>구분</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -123,6 +123,214 @@
   <si>
     <t>관리자 메인화면</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/index.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조주영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/list.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/register.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 등록 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 리스트 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 유형선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/member/join.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 유형 선택 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조주영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 약관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/member/signup.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 약관 동의 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 회원 가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/member/register.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 회원 가입 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매자 회원 가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/member/registerSeller.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매자 회원 가입 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 메인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 메인화면 / CS 최신글 받아오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/productDelete.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 단일 삭제 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 단일 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 다중 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 다중 삭제 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/productModify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 정보 수정 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 등록 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/member/login.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/member/logout.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 회원 가입 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조주영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매자 회원 가입 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 중복 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/member/uidCheck.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 중복 확인 체크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -152,12 +360,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -172,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,6 +402,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,16 +692,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -493,108 +723,417 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2022/12/28 API 일부 수정
</commit_message>
<xml_diff>
--- a/API/API 설계 조주영.xlsx
+++ b/API/API 설계 조주영.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
   <si>
     <t>구분</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -141,10 +141,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Kmarket/admin/list.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상품 목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -153,10 +149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Kmarket/admin/register.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상품 등록 화면</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -245,10 +237,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Kmarket/admin/productDelete.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상품 단일 삭제 처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -273,10 +261,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Kmarket/admin/productModify.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상품 정보 수정 처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -337,10 +321,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Kmarket/admin/category.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -370,6 +350,30 @@
   </si>
   <si>
     <t>조주영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/product/list.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/product/productDelete.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/product/productDelete.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/product/productModify.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/product/register.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Kmarket/admin/product/category.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -734,14 +738,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -873,7 +877,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>27</v>
@@ -882,7 +886,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>29</v>
@@ -890,16 +894,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>29</v>
@@ -907,16 +911,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>29</v>
@@ -924,16 +928,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>29</v>
@@ -941,16 +945,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>29</v>
@@ -958,16 +962,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>29</v>
@@ -975,16 +979,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>29</v>
@@ -992,24 +996,24 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1018,16 +1022,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>29</v>
@@ -1035,16 +1039,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>29</v>
@@ -1052,50 +1056,50 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E22" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>29</v>
@@ -1103,33 +1107,33 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>29</v>
@@ -1137,16 +1141,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>29</v>
@@ -1154,16 +1158,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>29</v>
@@ -1171,16 +1175,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>29</v>
@@ -1188,19 +1192,19 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>